<commit_message>
updated KARMEN DPE P1/P2
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KARMEN_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KARMEN_P1.xlsx
@@ -530,7 +530,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Age at exposure measure</t>
+          <t>Age at exposure measure [years]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Physical activity from questionnaire data</t>
+          <t>Physical activity from questionnaire data [MET-hr/day]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -665,7 +665,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>MET-min/Wo</t>
+          <t>MET-min/week</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -705,22 +705,32 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>__BLANK__</t>
+          <t>impossible</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>paste</t>
+          <t>impossible</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>impossible</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Mean Activity energy expenditure (AEE) assessed by Actiheart</t>
+          <t>unavailable</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>impossible</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>unavailable</t>
         </is>
       </c>
     </row>

</xml_diff>